<commit_message>
finish xls and ready to rebuild the circuit
</commit_message>
<xml_diff>
--- a/mips_i.xlsx
+++ b/mips_i.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tangyifeng/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tangyifeng/CPU/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="500" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="178">
   <si>
     <t>指令</t>
     <rPh sb="0" eb="1">
@@ -309,10 +309,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PC+8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Jr</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -341,10 +337,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>imm&lt;&lt;16</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Rt</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -353,43 +345,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>PC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>NPC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>NPC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>PC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Offset</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NPC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NPC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4/Offset&lt;&lt;2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rf.D1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4/Offset&lt;&lt;2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -438,17 +410,6 @@
   </si>
   <si>
     <t>PC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Offset(Imi)</t>
-  </si>
-  <si>
-    <t>Offset(Imi)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4/Offset(Imi2)&lt;&lt;2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -501,6 +462,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>I</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -509,6 +478,22 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>I</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>R</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -517,115 +502,262 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>I</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>R</t>
+    <t>B1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SIZE0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R1#1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R1#0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W#1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W#0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Din#1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Din#0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SIZE1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rs(00)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rt(01)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$v0(10)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rt(0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0(1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R2#</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rd(00)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rt(01)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>31(10)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU(00)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DM(01)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC+8(10)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>imm&lt;&lt;16(11)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rf.D2(00)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Imi(01)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sha(10)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Imi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Imi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10(11)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC_CON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IN1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Imi1&lt;&lt;2</t>
+  </si>
+  <si>
+    <t>Imi1&lt;&lt;2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Imi1&lt;&lt;2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Imi2&lt;&lt;2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC+NPC_CON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IN2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC+NPC_CON(00)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Imi2&lt;&lt;2(01)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rf.D1(10)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R(00)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I(01)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J(10)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>I</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>I</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>I</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>J</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>J</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>I</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SIZE0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R1#1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R1#0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R2#1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R2#0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>W#1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>W#0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Din#1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Din#0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Off1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Off0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SIZE1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rs(00)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rt(01)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>$v0(10)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -762,7 +894,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -773,25 +905,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="24" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="24" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -801,6 +921,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1080,10 +1209,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q61"/>
+  <dimension ref="A1:T61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="R50" sqref="R50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -1091,38 +1220,43 @@
     <col min="14" max="14" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
       <c r="B1" s="7"/>
       <c r="C1" s="6"/>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17" t="s">
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="17"/>
-      <c r="M1" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="N1" s="19"/>
-      <c r="O1" s="17" t="s">
-        <v>106</v>
+      <c r="L1" s="13"/>
+      <c r="M1" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" s="15"/>
+      <c r="O1" s="16" t="s">
+        <v>146</v>
       </c>
       <c r="P1" s="17"/>
-      <c r="Q1" s="15" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="Q1" s="18"/>
+      <c r="R1" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="S1" s="13"/>
+      <c r="T1" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1151,7 +1285,7 @@
         <v>8</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>9</v>
@@ -1160,48 +1294,57 @@
         <v>10</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>83</v>
+        <v>145</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>104</v>
+        <v>147</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q2" s="16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+        <v>154</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>21</v>
+        <v>128</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>22</v>
+        <v>132</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>16</v>
+        <v>135</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>24</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>38</v>
+        <v>139</v>
       </c>
       <c r="J3">
         <v>101</v>
@@ -1209,27 +1352,34 @@
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
       <c r="M3" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="N3" s="10">
+        <v>79</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="O3" s="8">
         <v>4</v>
       </c>
-      <c r="O3" s="8">
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="R3" s="8">
         <v>0</v>
       </c>
-      <c r="P3" s="8">
+      <c r="S3" s="8">
         <v>100000</v>
       </c>
-      <c r="Q3" s="15" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="T3" s="8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>18</v>
@@ -1239,7 +1389,7 @@
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>19</v>
+        <v>133</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>23</v>
@@ -1248,7 +1398,7 @@
         <v>24</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>25</v>
+        <v>140</v>
       </c>
       <c r="J4">
         <v>101</v>
@@ -1256,25 +1406,32 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="N4" s="11">
+        <v>82</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="O4" s="2">
         <v>4</v>
       </c>
-      <c r="O4" s="2">
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R4" s="2">
         <v>1000</v>
       </c>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="15" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="S4" s="2"/>
+      <c r="T4" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>18</v>
@@ -1301,25 +1458,32 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="N5" s="11">
+        <v>82</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="O5" s="2">
         <v>4</v>
       </c>
-      <c r="O5" s="2">
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="R5" s="2">
         <v>1001</v>
       </c>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="S5" s="2"/>
+      <c r="T5" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>15</v>
@@ -1348,27 +1512,34 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="N6" s="11">
+        <v>82</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="O6" s="2">
         <v>4</v>
       </c>
-      <c r="O6" s="2">
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="R6" s="2">
         <v>0</v>
       </c>
-      <c r="P6" s="2">
+      <c r="S6" s="2">
         <v>100001</v>
       </c>
-      <c r="Q6" s="15" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="T6" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>29</v>
@@ -1397,33 +1568,40 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="N7" s="11">
+        <v>82</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="O7" s="2">
         <v>4</v>
       </c>
-      <c r="O7" s="2">
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="R7" s="2">
         <v>0</v>
       </c>
-      <c r="P7" s="2">
+      <c r="S7" s="2">
         <v>100100</v>
       </c>
-      <c r="Q7" s="15" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="T7" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
@@ -1444,25 +1622,32 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="N8" s="11">
+        <v>82</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="O8" s="2">
         <v>4</v>
       </c>
-      <c r="O8" s="2">
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="R8" s="2">
         <v>1100</v>
       </c>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="S8" s="2"/>
+      <c r="T8" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>18</v>
@@ -1481,7 +1666,7 @@
         <v>37</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>40</v>
+        <v>141</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1489,27 +1674,34 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="N9" s="11">
+        <v>82</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="O9" s="2">
         <v>4</v>
       </c>
-      <c r="O9" s="2">
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R9" s="2">
         <v>0</v>
       </c>
-      <c r="P9" s="2">
+      <c r="S9" s="2">
         <v>0</v>
       </c>
-      <c r="Q9" s="15" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="T9" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>18</v>
@@ -1536,27 +1728,34 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="N10" s="11">
+        <v>82</v>
+      </c>
+      <c r="N10" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="O10" s="2">
         <v>4</v>
       </c>
-      <c r="O10" s="2">
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="R10" s="2">
         <v>0</v>
       </c>
-      <c r="P10" s="2">
+      <c r="S10" s="2">
         <v>11</v>
       </c>
-      <c r="Q10" s="15" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="T10" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>18</v>
@@ -1583,27 +1782,34 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="N11" s="11">
+        <v>82</v>
+      </c>
+      <c r="N11" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="O11" s="2">
         <v>4</v>
       </c>
-      <c r="O11" s="2">
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="R11" s="2">
         <v>0</v>
       </c>
-      <c r="P11" s="2">
+      <c r="S11" s="2">
         <v>10</v>
       </c>
-      <c r="Q11" s="15" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="T11" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>15</v>
@@ -1632,27 +1838,34 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="N12" s="11">
+        <v>82</v>
+      </c>
+      <c r="N12" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="O12" s="2">
         <v>4</v>
       </c>
-      <c r="O12" s="2">
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R12" s="2">
         <v>0</v>
       </c>
-      <c r="P12" s="2">
+      <c r="S12" s="2">
         <v>100010</v>
       </c>
-      <c r="Q12" s="15" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="T12" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>15</v>
@@ -1681,27 +1894,34 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="N13" s="11">
+        <v>82</v>
+      </c>
+      <c r="N13" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="O13" s="2">
         <v>4</v>
       </c>
-      <c r="O13" s="2">
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="R13" s="2">
         <v>0</v>
       </c>
-      <c r="P13" s="2">
+      <c r="S13" s="2">
         <v>100101</v>
       </c>
-      <c r="Q13" s="15" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="T13" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>18</v>
@@ -1728,25 +1948,32 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="N14" s="11">
+        <v>82</v>
+      </c>
+      <c r="N14" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="O14" s="2">
         <v>4</v>
       </c>
-      <c r="O14" s="2">
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R14" s="2">
         <v>1101</v>
       </c>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="15" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="S14" s="2"/>
+      <c r="T14" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>15</v>
@@ -1775,27 +2002,34 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="N15" s="11">
+        <v>82</v>
+      </c>
+      <c r="N15" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="O15" s="2">
         <v>4</v>
       </c>
-      <c r="O15" s="2">
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R15" s="2">
         <v>0</v>
       </c>
-      <c r="P15" s="2">
+      <c r="S15" s="2">
         <v>100111</v>
       </c>
-      <c r="Q15" s="15" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="T15" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>18</v>
@@ -1808,13 +2042,13 @@
         <v>48</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>49</v>
+        <v>136</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>36</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>101</v>
+        <v>142</v>
       </c>
       <c r="J16">
         <v>101</v>
@@ -1824,25 +2058,32 @@
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="N16" s="11">
+        <v>82</v>
+      </c>
+      <c r="N16" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="O16" s="2">
         <v>4</v>
       </c>
-      <c r="O16" s="2">
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="R16" s="2">
         <v>100011</v>
       </c>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="S16" s="2"/>
+      <c r="T16" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>18</v>
@@ -1859,7 +2100,7 @@
         <v>51</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>100</v>
+        <v>143</v>
       </c>
       <c r="J17">
         <v>101</v>
@@ -1871,25 +2112,32 @@
         <v>52</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="N17" s="11">
+        <v>82</v>
+      </c>
+      <c r="N17" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="O17" s="2">
         <v>4</v>
       </c>
-      <c r="O17" s="2">
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="R17" s="2">
         <v>101011</v>
       </c>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="15" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="S17" s="2"/>
+      <c r="T17" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>18</v>
@@ -1914,25 +2162,34 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="N18" s="11" t="s">
-        <v>87</v>
+        <v>79</v>
+      </c>
+      <c r="N18" s="10" t="s">
+        <v>152</v>
       </c>
       <c r="O18" s="2">
+        <v>4</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R18" s="2">
         <v>100</v>
       </c>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="15" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="S18" s="2"/>
+      <c r="T18" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>18</v>
@@ -1957,25 +2214,34 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="N19" s="11" t="s">
-        <v>87</v>
+        <v>79</v>
+      </c>
+      <c r="N19" s="10" t="s">
+        <v>152</v>
       </c>
       <c r="O19" s="2">
+        <v>4</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="R19" s="2">
         <v>101</v>
       </c>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="15" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="S19" s="2"/>
+      <c r="T19" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>18</v>
@@ -2004,27 +2270,34 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="N20" s="11">
+        <v>82</v>
+      </c>
+      <c r="N20" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="O20" s="2">
         <v>4</v>
       </c>
-      <c r="O20" s="2">
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R20" s="2">
         <v>0</v>
       </c>
-      <c r="P20" s="2">
+      <c r="S20" s="2">
         <v>101010</v>
       </c>
-      <c r="Q20" s="15" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="T20" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>18</v>
@@ -2051,25 +2324,32 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="N21" s="11">
+        <v>82</v>
+      </c>
+      <c r="N21" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="O21" s="2">
         <v>4</v>
       </c>
-      <c r="O21" s="2">
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R21" s="2">
         <v>1010</v>
       </c>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="S21" s="2"/>
+      <c r="T21" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>18</v>
@@ -2098,27 +2378,34 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="N22" s="11">
+        <v>82</v>
+      </c>
+      <c r="N22" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="O22" s="2">
         <v>4</v>
       </c>
-      <c r="O22" s="2">
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R22" s="2">
         <v>0</v>
       </c>
-      <c r="P22" s="2">
+      <c r="S22" s="2">
         <v>101011</v>
       </c>
-      <c r="Q22" s="15" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="T22" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>67</v>
@@ -2132,67 +2419,73 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="N23" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="O23" s="2">
+        <v>79</v>
+      </c>
+      <c r="N23" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2">
         <v>10</v>
       </c>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="15" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="S23" s="2"/>
+      <c r="T23" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="14">
-        <v>31</v>
+      <c r="F24" s="12" t="s">
+        <v>134</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>70</v>
+        <v>137</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="N24" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="O24" s="2">
+        <v>79</v>
+      </c>
+      <c r="N24" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2">
         <v>11</v>
       </c>
-      <c r="P24" s="2"/>
-      <c r="Q24" s="15" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="S24" s="2"/>
+      <c r="T24" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -2202,33 +2495,36 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="N25" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="O25" s="2">
+        <v>83</v>
+      </c>
+      <c r="N25" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2">
         <v>0</v>
       </c>
-      <c r="P25" s="2">
+      <c r="S25" s="2">
         <v>1000</v>
       </c>
-      <c r="Q25" s="15" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="T25" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -2236,8 +2532,8 @@
       <c r="H26" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I26" s="11">
-        <v>10</v>
+      <c r="I26" s="10" t="s">
+        <v>144</v>
       </c>
       <c r="J26">
         <v>110</v>
@@ -2245,25 +2541,34 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="N26" s="11">
+        <v>79</v>
+      </c>
+      <c r="N26" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="O26" s="2">
         <v>4</v>
       </c>
-      <c r="O26" s="2">
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="R26" s="2">
         <v>0</v>
       </c>
-      <c r="P26" s="2">
+      <c r="S26" s="2">
         <v>1100</v>
       </c>
-      <c r="Q26" s="15"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="T26" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>18</v>
@@ -2290,61 +2595,75 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="N27" s="11">
+        <v>79</v>
+      </c>
+      <c r="N27" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="O27" s="2">
         <v>4</v>
       </c>
-      <c r="O27" s="2">
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="R27" s="2">
         <v>1110</v>
       </c>
-      <c r="P27" s="2"/>
-      <c r="Q27" s="15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="S27" s="2"/>
+      <c r="T27" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>78</v>
+        <v>138</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
       <c r="M28" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="N28" s="11">
+        <v>79</v>
+      </c>
+      <c r="N28" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="O28" s="2">
         <v>4</v>
       </c>
-      <c r="O28" s="2">
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="R28" s="2">
         <v>1111</v>
       </c>
-      <c r="P28" s="2"/>
-      <c r="Q28" s="15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="S28" s="2"/>
+      <c r="T28" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>1</v>
@@ -2363,7 +2682,7 @@
         <v>36</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>100</v>
+        <v>143</v>
       </c>
       <c r="J29">
         <v>101</v>
@@ -2373,34 +2692,41 @@
       </c>
       <c r="L29" s="2"/>
       <c r="M29" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="N29" s="11">
+        <v>79</v>
+      </c>
+      <c r="N29" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="O29" s="2">
         <v>4</v>
       </c>
-      <c r="O29">
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="R29">
         <v>100001</v>
       </c>
-      <c r="P29" s="2"/>
-      <c r="Q29" s="15" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="S29" s="2"/>
+      <c r="T29" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E30" s="13">
-        <v>0</v>
+        <v>77</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>129</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -2408,7 +2734,7 @@
         <v>55</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J30">
         <v>1011</v>
@@ -2416,65 +2742,83 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="N30" s="12" t="s">
-        <v>90</v>
+        <v>79</v>
+      </c>
+      <c r="N30" s="10" t="s">
+        <v>152</v>
       </c>
       <c r="O30" s="1">
-        <v>1</v>
-      </c>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="R30" s="1">
+        <v>1</v>
+      </c>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="J31" s="4"/>
       <c r="K31" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="15"/>
-    </row>
-    <row r="32" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+      <c r="O31" s="4">
+        <v>4</v>
+      </c>
+      <c r="P31" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q31" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="4"/>
+    </row>
+    <row r="32" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -2488,219 +2832,381 @@
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="E33" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="G33" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>135</v>
-      </c>
       <c r="H33" s="4" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>139</v>
+        <v>169</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="O33" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.15">
+        <v>116</v>
+      </c>
+      <c r="P33" s="3"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A34" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="O35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="O36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A37" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A38" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A39" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="K39">
+        <v>1</v>
+      </c>
+      <c r="O39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A40" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="J40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A41" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="J41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A42" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="J42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A43" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A44" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A45" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="K45">
+        <v>1</v>
+      </c>
+      <c r="O45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A47" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+      <c r="K47">
+        <v>1</v>
+      </c>
+      <c r="O47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A48" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="K48">
+        <v>1</v>
+      </c>
+      <c r="O48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A49" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="O49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A50" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="O50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A51" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A52" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="K52">
+        <v>1</v>
+      </c>
+      <c r="O52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A53" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A54" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="M54">
+        <v>1</v>
+      </c>
+      <c r="N54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A55" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="H55">
+        <v>1</v>
+      </c>
+      <c r="M55">
+        <v>1</v>
+      </c>
+      <c r="N55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A56" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
+        <v>70</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="L56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A57" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="J57">
+        <v>1</v>
+      </c>
+      <c r="O57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A58" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="K58">
+        <v>1</v>
+      </c>
+      <c r="O58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A59" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A58" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A59" s="2" t="s">
+      <c r="F59">
+        <v>1</v>
+      </c>
+      <c r="H59">
+        <v>1</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+      <c r="O59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A60" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A60" s="2" t="s">
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+      <c r="K60">
+        <v>1</v>
+      </c>
+      <c r="O60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="C61">
         <v>1</v>
       </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="O61">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="O1:Q1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
delete the old one but something is not going well
</commit_message>
<xml_diff>
--- a/mips_i.xlsx
+++ b/mips_i.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="206">
   <si>
     <t>指令</t>
     <rPh sb="0" eb="1">
@@ -758,6 +758,118 @@
   </si>
   <si>
     <t>I</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add(1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddI(2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddIU(3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddU(4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>And(5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AndI(6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SLL(7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRA(8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRL(9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sub(10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Or(11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OrI(12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nor(13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LoadW(14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StoreW(15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beq(16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bne(17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slt(18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slti(19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sltu(20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jump(21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jal(22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jr(23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Syscall(24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Xori(25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lui(26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lh(27</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bltz(28</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1212,7 +1324,7 @@
   <dimension ref="A1:T61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="R50" sqref="R50"/>
+      <selection activeCell="N54" sqref="N54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -2880,13 +2992,13 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A34" s="8" t="s">
-        <v>14</v>
+        <v>178</v>
       </c>
       <c r="G34" s="3"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
-        <v>17</v>
+        <v>179</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -2900,7 +3012,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
-        <v>26</v>
+        <v>180</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -2914,17 +3026,17 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A37" s="2" t="s">
-        <v>27</v>
+        <v>181</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A38" s="2" t="s">
-        <v>28</v>
+        <v>182</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A39" s="2" t="s">
-        <v>30</v>
+        <v>183</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -2938,7 +3050,7 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A40" s="2" t="s">
-        <v>31</v>
+        <v>184</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -2949,7 +3061,7 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A41" s="2" t="s">
-        <v>41</v>
+        <v>185</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -2960,7 +3072,7 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A42" s="2" t="s">
-        <v>42</v>
+        <v>186</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -2971,17 +3083,17 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A43" s="2" t="s">
-        <v>43</v>
+        <v>187</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A44" s="2" t="s">
-        <v>44</v>
+        <v>188</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A45" s="2" t="s">
-        <v>45</v>
+        <v>189</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -2995,12 +3107,12 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
-        <v>46</v>
+        <v>190</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A47" s="2" t="s">
-        <v>47</v>
+        <v>191</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -3017,7 +3129,7 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A48" s="2" t="s">
-        <v>50</v>
+        <v>192</v>
       </c>
       <c r="G48">
         <v>1</v>
@@ -3031,7 +3143,7 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A49" s="2" t="s">
-        <v>53</v>
+        <v>193</v>
       </c>
       <c r="G49">
         <v>1</v>
@@ -3042,7 +3154,7 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A50" s="2" t="s">
-        <v>56</v>
+        <v>194</v>
       </c>
       <c r="G50">
         <v>1</v>
@@ -3053,12 +3165,12 @@
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A51" s="2" t="s">
-        <v>60</v>
+        <v>195</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A52" s="2" t="s">
-        <v>61</v>
+        <v>196</v>
       </c>
       <c r="F52">
         <v>1</v>
@@ -3072,12 +3184,12 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A53" s="2" t="s">
-        <v>66</v>
+        <v>197</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A54" s="2" t="s">
-        <v>68</v>
+        <v>198</v>
       </c>
       <c r="G54">
         <v>1</v>
@@ -3091,7 +3203,7 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A55" s="2" t="s">
-        <v>69</v>
+        <v>199</v>
       </c>
       <c r="H55">
         <v>1</v>
@@ -3105,7 +3217,7 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A56" s="2" t="s">
-        <v>70</v>
+        <v>200</v>
       </c>
       <c r="G56">
         <v>1</v>
@@ -3116,7 +3228,7 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A57" s="2" t="s">
-        <v>72</v>
+        <v>201</v>
       </c>
       <c r="B57">
         <v>1</v>
@@ -3133,7 +3245,7 @@
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A58" s="2" t="s">
-        <v>97</v>
+        <v>202</v>
       </c>
       <c r="F58">
         <v>1</v>
@@ -3150,7 +3262,7 @@
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A59" s="2" t="s">
-        <v>73</v>
+        <v>203</v>
       </c>
       <c r="F59">
         <v>1</v>
@@ -3167,7 +3279,7 @@
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A60" s="2" t="s">
-        <v>74</v>
+        <v>204</v>
       </c>
       <c r="F60">
         <v>1</v>
@@ -3184,7 +3296,7 @@
     </row>
     <row r="61" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>75</v>
+        <v>205</v>
       </c>
       <c r="C61">
         <v>1</v>

</xml_diff>